<commit_message>
Updated the results to contain the new encryption graph
</commit_message>
<xml_diff>
--- a/documents/encryption_test_results.xlsx
+++ b/documents/encryption_test_results.xlsx
@@ -9,15 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
   <si>
     <t>Successful decryption time (ms)</t>
   </si>
@@ -26,6 +23,9 @@
   </si>
   <si>
     <t>Unsuccessful decryption time (ms)</t>
+  </si>
+  <si>
+    <t>Number messages</t>
   </si>
 </sst>
 </file>
@@ -98,10 +98,2742 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sucessful vs Unsucessful Decryption Time (ms)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sucessful</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$1:$A$51</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$2:$A$51</c:f>
+              <c:strCache>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>840</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$C$2:$C$51</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$C$3:$C$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>10.686</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.135999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.4090000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.8209999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.3729999999999993</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.2059999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.8259999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.6890000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.6420000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.6719999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.6890000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.0169999999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.74</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.734</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.7130000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.7759999999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.665</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.72</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.7229999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.7169999999999996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.6420000000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.6790000000000003</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.6660000000000004</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.7130000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.77</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.7169999999999996</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.9219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7.9619999999999997</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8.2780000000000005</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.5890000000000004</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7.9850000000000003</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.7750000000000004</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7.8049999999999997</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7.7030000000000003</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.6879999999999997</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.694</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.7469999999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.7430000000000003</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7.65</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7.6470000000000002</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7.6669999999999998</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.69</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7.9610000000000003</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7.67</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>7.7539999999999996</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>7.6639999999999997</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>7.6660000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Unsucessful</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$1:$A$51</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$2:$A$51</c:f>
+              <c:strCache>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>840</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$D$2:$D$51</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$D$3:$D$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>10.381</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.7430000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.0820000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.6329999999999991</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.3789999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.9180000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.7880000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.8659999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.681</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.7370000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.7409999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.734</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.74</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.734</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.7679999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.673</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.6989999999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.774</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.7069999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.923</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.6989999999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.6929999999999996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.7350000000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.7549999999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.7640000000000002</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.72</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.6740000000000004</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.673</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.7629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8.2070000000000007</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8.1649999999999991</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.2360000000000007</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8.907</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.6849999999999996</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7.7160000000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7.8140000000000001</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.7130000000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>7.7439999999999998</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.7190000000000003</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>7.7619999999999996</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7.7619999999999996</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7.7080000000000002</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7.8230000000000004</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.681</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7.875</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7.7960000000000003</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>7.72</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>7.774</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>7.7279999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="321530920"/>
+        <c:axId val="326184640"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="321530920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Length</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of message (characters)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="326184640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="326184640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="7"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="321530920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Encryption time (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>0.374</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.20799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.153</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.14399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.14499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.14499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.14499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.14599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.14499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.14599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.14599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.14599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.157</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.157</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.14599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.14599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.14899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.192</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.161</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.159</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.158</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.14899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.152</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.153</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.14899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.151</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="325328096"/>
+        <c:axId val="325327312"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="325328096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="325327312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="325327312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="325328096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>157162</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>461962</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D51" totalsRowShown="0" tableBorderDxfId="0">
   <tableColumns count="4">
-    <tableColumn id="1" name=" "/>
+    <tableColumn id="1" name="Number messages"/>
     <tableColumn id="2" name="Encryption time (ms)"/>
     <tableColumn id="3" name="Successful decryption time (ms)"/>
     <tableColumn id="4" name="Unsuccessful decryption time (ms)"/>
@@ -400,27 +3132,29 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="4" width="10" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -438,7 +3172,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1">
+        <f>A2 + 20</f>
+        <v>40</v>
+      </c>
       <c r="B3" s="1">
         <v>0.20799999999999999</v>
       </c>
@@ -450,7 +3187,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <f t="shared" ref="A4:A51" si="0">A3 + 20</f>
+        <v>60</v>
+      </c>
       <c r="B4" s="1">
         <v>0.19</v>
       </c>
@@ -462,7 +3202,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
       <c r="B5" s="1">
         <v>0.17699999999999999</v>
       </c>
@@ -474,7 +3217,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="B6">
@@ -488,6 +3232,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
       <c r="B7">
         <v>0.16</v>
       </c>
@@ -499,6 +3247,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
       <c r="B8">
         <v>0.153</v>
       </c>
@@ -510,6 +3262,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
       <c r="B9">
         <v>0.14699999999999999</v>
       </c>
@@ -521,6 +3277,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
       <c r="B10">
         <v>0.14699999999999999</v>
       </c>
@@ -532,7 +3292,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="B11">
@@ -546,6 +3307,10 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>220</v>
+      </c>
       <c r="B12">
         <v>0.14399999999999999</v>
       </c>
@@ -557,6 +3322,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
       <c r="B13">
         <v>0.14799999999999999</v>
       </c>
@@ -568,6 +3337,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
       <c r="B14">
         <v>0.14499999999999999</v>
       </c>
@@ -579,6 +3352,10 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
       <c r="B15">
         <v>0.14499999999999999</v>
       </c>
@@ -590,7 +3367,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="B16">
@@ -604,6 +3382,10 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>320</v>
+      </c>
       <c r="B17">
         <v>0.14599999999999999</v>
       </c>
@@ -615,6 +3397,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>340</v>
+      </c>
       <c r="B18">
         <v>0.14499999999999999</v>
       </c>
@@ -626,6 +3412,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
       <c r="B19">
         <v>0.14699999999999999</v>
       </c>
@@ -637,6 +3427,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>380</v>
+      </c>
       <c r="B20">
         <v>0.14599999999999999</v>
       </c>
@@ -648,7 +3442,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
         <v>400</v>
       </c>
       <c r="B21">
@@ -662,6 +3457,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>420</v>
+      </c>
       <c r="B22">
         <v>0.14599999999999999</v>
       </c>
@@ -673,6 +3472,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <f t="shared" si="0"/>
+        <v>440</v>
+      </c>
       <c r="B23">
         <v>0.15</v>
       </c>
@@ -684,6 +3487,10 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <f t="shared" si="0"/>
+        <v>460</v>
+      </c>
       <c r="B24">
         <v>0.14599999999999999</v>
       </c>
@@ -695,6 +3502,10 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
       <c r="B25">
         <v>0.157</v>
       </c>
@@ -706,7 +3517,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="1">
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="B26">
@@ -720,6 +3532,10 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>520</v>
+      </c>
       <c r="B27">
         <v>0.14699999999999999</v>
       </c>
@@ -731,6 +3547,10 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <f t="shared" si="0"/>
+        <v>540</v>
+      </c>
       <c r="B28">
         <v>0.14599999999999999</v>
       </c>
@@ -742,6 +3562,10 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <f t="shared" si="0"/>
+        <v>560</v>
+      </c>
       <c r="B29">
         <v>0.14599999999999999</v>
       </c>
@@ -753,6 +3577,10 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <f t="shared" si="0"/>
+        <v>580</v>
+      </c>
       <c r="B30">
         <v>0.14899999999999999</v>
       </c>
@@ -764,7 +3592,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="1">
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="B31">
@@ -778,6 +3607,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <f t="shared" si="0"/>
+        <v>620</v>
+      </c>
       <c r="B32">
         <v>0.14699999999999999</v>
       </c>
@@ -789,6 +3622,10 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <f t="shared" si="0"/>
+        <v>640</v>
+      </c>
       <c r="B33">
         <v>0.192</v>
       </c>
@@ -800,6 +3637,10 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <f t="shared" si="0"/>
+        <v>660</v>
+      </c>
       <c r="B34">
         <v>0.161</v>
       </c>
@@ -811,6 +3652,10 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <f t="shared" si="0"/>
+        <v>680</v>
+      </c>
       <c r="B35">
         <v>0.159</v>
       </c>
@@ -822,7 +3667,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="1">
+        <f t="shared" si="0"/>
         <v>700</v>
       </c>
       <c r="B36">
@@ -836,6 +3682,10 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <f t="shared" si="0"/>
+        <v>720</v>
+      </c>
       <c r="B37">
         <v>0.14699999999999999</v>
       </c>
@@ -847,6 +3697,10 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <f t="shared" si="0"/>
+        <v>740</v>
+      </c>
       <c r="B38">
         <v>0.14899999999999999</v>
       </c>
@@ -858,6 +3712,10 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <f t="shared" si="0"/>
+        <v>760</v>
+      </c>
       <c r="B39">
         <v>0.14699999999999999</v>
       </c>
@@ -869,6 +3727,10 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <f t="shared" si="0"/>
+        <v>780</v>
+      </c>
       <c r="B40">
         <v>0.14799999999999999</v>
       </c>
@@ -880,7 +3742,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="1">
+        <f t="shared" si="0"/>
         <v>800</v>
       </c>
       <c r="B41">
@@ -894,6 +3757,10 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <f t="shared" si="0"/>
+        <v>820</v>
+      </c>
       <c r="B42">
         <v>0.14799999999999999</v>
       </c>
@@ -905,6 +3772,10 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <f t="shared" si="0"/>
+        <v>840</v>
+      </c>
       <c r="B43">
         <v>0.14699999999999999</v>
       </c>
@@ -916,6 +3787,10 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <f t="shared" si="0"/>
+        <v>860</v>
+      </c>
       <c r="B44">
         <v>0.15</v>
       </c>
@@ -927,6 +3802,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <f t="shared" si="0"/>
+        <v>880</v>
+      </c>
       <c r="B45">
         <v>0.14799999999999999</v>
       </c>
@@ -938,7 +3817,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="1">
+        <f t="shared" si="0"/>
         <v>900</v>
       </c>
       <c r="B46">
@@ -952,6 +3832,10 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <f t="shared" si="0"/>
+        <v>920</v>
+      </c>
       <c r="B47">
         <v>0.14899999999999999</v>
       </c>
@@ -963,6 +3847,10 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <f t="shared" si="0"/>
+        <v>940</v>
+      </c>
       <c r="B48">
         <v>0.14799999999999999</v>
       </c>
@@ -974,6 +3862,10 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <f t="shared" si="0"/>
+        <v>960</v>
+      </c>
       <c r="B49">
         <v>0.14799999999999999</v>
       </c>
@@ -985,6 +3877,10 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <f t="shared" si="0"/>
+        <v>980</v>
+      </c>
       <c r="B50">
         <v>0.14799999999999999</v>
       </c>
@@ -996,7 +3892,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="1">
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="B51">
@@ -1011,8 +3908,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished the results section on encryption + decryption
</commit_message>
<xml_diff>
--- a/documents/encryption_test_results.xlsx
+++ b/documents/encryption_test_results.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\projects\Anonychat\documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="90" windowWidth="9555" windowHeight="7755"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Successful decryption time (ms)</t>
   </si>
@@ -26,6 +31,21 @@
   </si>
   <si>
     <t>Number messages</t>
+  </si>
+  <si>
+    <t>Encryption Time</t>
+  </si>
+  <si>
+    <t>Decryption Time</t>
+  </si>
+  <si>
+    <t>Average (ms)</t>
+  </si>
+  <si>
+    <t>Max (ms)</t>
+  </si>
+  <si>
+    <t>Min (ms)</t>
   </si>
 </sst>
 </file>
@@ -871,7 +891,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -880,11 +899,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="321530920"/>
-        <c:axId val="326184640"/>
+        <c:axId val="215461840"/>
+        <c:axId val="215455960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="321530920"/>
+        <c:axId val="215461840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -988,7 +1007,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="326184640"/>
+        <c:crossAx val="215455960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -996,7 +1015,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="326184640"/>
+        <c:axId val="215455960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="7"/>
@@ -1109,7 +1128,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321530920"/>
+        <c:crossAx val="215461840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1437,11 +1456,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="325328096"/>
-        <c:axId val="325327312"/>
+        <c:axId val="215460664"/>
+        <c:axId val="215455568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="325328096"/>
+        <c:axId val="215460664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1514,7 +1533,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325327312"/>
+        <c:crossAx val="215455568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1522,7 +1541,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="325327312"/>
+        <c:axId val="215455568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1604,7 +1623,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="325328096"/>
+        <c:crossAx val="215460664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2769,16 +2788,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>323849</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>90488</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>138113</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>390524</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2799,16 +2818,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>157162</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>557212</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>461962</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>252412</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3129,10 +3148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="G21" sqref="G21:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3141,6 +3160,9 @@
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3381,7 +3403,7 @@
         <v>7.734</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>320</v>
@@ -3396,7 +3418,7 @@
         <v>7.7679999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>340</v>
@@ -3411,7 +3433,7 @@
         <v>7.673</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>360</v>
@@ -3426,7 +3448,7 @@
         <v>7.6989999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>380</v>
@@ -3441,7 +3463,7 @@
         <v>7.774</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>400</v>
@@ -3455,8 +3477,17 @@
       <c r="D21">
         <v>7.7069999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>420</v>
@@ -3470,8 +3501,23 @@
       <c r="D22">
         <v>7.923</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <f>AVERAGE(Table1[Encryption time (ms)])</f>
+        <v>0.15747999999999998</v>
+      </c>
+      <c r="I22">
+        <f>MAX(Table1[Encryption time (ms)])</f>
+        <v>0.374</v>
+      </c>
+      <c r="J22">
+        <f>MIN(Table1[Encryption time (ms)])</f>
+        <v>0.14399999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>440</v>
@@ -3485,8 +3531,23 @@
       <c r="D23">
         <v>7.6989999999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23">
+        <f>AVERAGE(Table1[Successful decryption time (ms)])</f>
+        <v>8.1296199999999992</v>
+      </c>
+      <c r="I23">
+        <f>MAX(Table1[Successful decryption time (ms)])</f>
+        <v>14.68</v>
+      </c>
+      <c r="J23">
+        <f>MIN(Table1[Successful decryption time (ms)])</f>
+        <v>7.6420000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>460</v>
@@ -3501,7 +3562,7 @@
         <v>7.6929999999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>480</v>
@@ -3516,7 +3577,7 @@
         <v>7.7350000000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>500</v>
@@ -3531,7 +3592,7 @@
         <v>7.7549999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>520</v>
@@ -3546,7 +3607,7 @@
         <v>7.7640000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>540</v>
@@ -3561,7 +3622,7 @@
         <v>7.72</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>560</v>
@@ -3576,7 +3637,7 @@
         <v>7.6740000000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>580</v>
@@ -3591,7 +3652,7 @@
         <v>7.673</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>600</v>
@@ -3606,7 +3667,7 @@
         <v>7.7629999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>620</v>

</xml_diff>

<commit_message>
Added the latency test results
</commit_message>
<xml_diff>
--- a/documents/encryption_test_results.xlsx
+++ b/documents/encryption_test_results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Successful decryption time (ms)</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Min (ms)</t>
+  </si>
+  <si>
+    <t>AVG (SUC - UNSUC)</t>
+  </si>
+  <si>
+    <t>SUC - unSUC</t>
   </si>
 </sst>
 </file>
@@ -88,7 +94,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1224,6 +1233,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Encryption time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs Message Length</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1286,32 +1325,204 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$1:$A$51</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$2:$A$51</c:f>
+              <c:strCache>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>840</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$51</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$2:$B$51</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$3:$B$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="0">
-                  <c:v>0.374</c:v>
+                  <c:v>0.20799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20799999999999999</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19</c:v>
+                  <c:v>0.17699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17699999999999999</c:v>
+                  <c:v>0.17199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17199999999999999</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16</c:v>
+                  <c:v>0.153</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.153</c:v>
+                  <c:v>0.14699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.14699999999999999</c:v>
@@ -1320,13 +1531,13 @@
                   <c:v>0.14699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.14699999999999999</c:v>
+                  <c:v>0.14399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.14399999999999999</c:v>
+                  <c:v>0.14799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.14799999999999999</c:v>
+                  <c:v>0.14499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.14499999999999999</c:v>
@@ -1335,100 +1546,100 @@
                   <c:v>0.14499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>0.14599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>0.14499999999999999</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>0.14599999999999999</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.14499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>0.14699999999999999</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>0.14599999999999999</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.14699999999999999</c:v>
-                </c:pt>
                 <c:pt idx="20">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>0.14599999999999999</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.15</c:v>
-                </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.14599999999999999</c:v>
+                  <c:v>0.157</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0.157</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.157</c:v>
+                  <c:v>0.14699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.14699999999999999</c:v>
+                  <c:v>0.14599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0.14599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.14599999999999999</c:v>
+                  <c:v>0.14899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.14899999999999999</c:v>
+                  <c:v>0.14699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0.14699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>0.192</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.161</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.159</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.158</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>0.14699999999999999</c:v>
                 </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.192</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.161</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.159</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.158</c:v>
-                </c:pt>
                 <c:pt idx="35">
+                  <c:v>0.14899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>0.14699999999999999</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.152</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.153</c:v>
+                </c:pt>
+                <c:pt idx="44">
                   <c:v>0.14899999999999999</c:v>
                 </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.14699999999999999</c:v>
-                </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="45">
                   <c:v>0.14799999999999999</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.152</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.14799999999999999</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.14699999999999999</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.14799999999999999</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.153</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.14899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>0.14799999999999999</c:v>
@@ -1437,9 +1648,6 @@
                   <c:v>0.14799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.14799999999999999</c:v>
-                </c:pt>
-                <c:pt idx="49">
                   <c:v>0.151</c:v>
                 </c:pt>
               </c:numCache>
@@ -1467,7 +1675,44 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Length of</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Message (characters)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.32877668416447942"/>
+              <c:y val="0.87868037328667248"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1497,6 +1742,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1544,6 +1790,7 @@
         <c:axId val="215455568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.13"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1562,6 +1809,36 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Encrpytion</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
@@ -2850,12 +3127,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D51" totalsRowShown="0" tableBorderDxfId="0">
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E51" totalsRowShown="0" tableBorderDxfId="1">
+  <tableColumns count="5">
     <tableColumn id="1" name="Number messages"/>
     <tableColumn id="2" name="Encryption time (ms)"/>
     <tableColumn id="3" name="Successful decryption time (ms)"/>
     <tableColumn id="4" name="Unsuccessful decryption time (ms)"/>
+    <tableColumn id="5" name="SUC - unSUC" dataDxfId="0">
+      <calculatedColumnFormula>C2 - D2</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3151,7 +3431,7 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21:J23"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3165,7 +3445,7 @@
     <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3178,8 +3458,11 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>20</v>
       </c>
@@ -3192,8 +3475,12 @@
       <c r="D2" s="1">
         <v>13.132</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <f t="shared" ref="E2:E33" si="0">C2 - D2</f>
+        <v>1.548</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>A2 + 20</f>
         <v>40</v>
@@ -3207,10 +3494,14 @@
       <c r="D3" s="1">
         <v>10.381</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>0.30499999999999972</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A51" si="0">A3 + 20</f>
+        <f t="shared" ref="A4:A51" si="1">A3 + 20</f>
         <v>60</v>
       </c>
       <c r="B4" s="1">
@@ -3222,10 +3513,14 @@
       <c r="D4" s="1">
         <v>9.7430000000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.39299999999999891</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="B5" s="1">
@@ -3237,10 +3532,14 @@
       <c r="D5" s="1">
         <v>9.0820000000000007</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.32699999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="B6">
@@ -3252,10 +3551,14 @@
       <c r="D6">
         <v>8.6329999999999991</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.18800000000000061</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="B7">
@@ -3267,10 +3570,14 @@
       <c r="D7">
         <v>8.3789999999999996</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>-6.0000000000002274E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>140</v>
       </c>
       <c r="B8">
@@ -3282,10 +3589,14 @@
       <c r="D8">
         <v>7.9180000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1.2879999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>160</v>
       </c>
       <c r="B9">
@@ -3297,10 +3608,14 @@
       <c r="D9">
         <v>7.7880000000000003</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>3.7999999999999368E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
       <c r="B10">
@@ -3312,10 +3627,14 @@
       <c r="D10">
         <v>7.8659999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>-0.1769999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="B11">
@@ -3327,10 +3646,14 @@
       <c r="D11">
         <v>7.681</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>-3.8999999999999702E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>220</v>
       </c>
       <c r="B12">
@@ -3342,10 +3665,14 @@
       <c r="D12">
         <v>7.7370000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>-6.5000000000000391E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="B13">
@@ -3357,10 +3684,14 @@
       <c r="D13">
         <v>7.7409999999999997</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>-5.1999999999999602E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>260</v>
       </c>
       <c r="B14">
@@ -3372,10 +3703,14 @@
       <c r="D14">
         <v>7.734</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.28299999999999947</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>280</v>
       </c>
       <c r="B15">
@@ -3387,10 +3722,14 @@
       <c r="D15">
         <v>7.74</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>300</v>
       </c>
       <c r="B16">
@@ -3402,10 +3741,14 @@
       <c r="D16">
         <v>7.734</v>
       </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>320</v>
       </c>
       <c r="B17">
@@ -3417,10 +3760,14 @@
       <c r="D17">
         <v>7.7679999999999998</v>
       </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>-6.7999999999999616E-2</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>340</v>
       </c>
       <c r="B18">
@@ -3432,10 +3779,14 @@
       <c r="D18">
         <v>7.673</v>
       </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>360</v>
       </c>
       <c r="B19">
@@ -3447,10 +3798,14 @@
       <c r="D19">
         <v>7.6989999999999998</v>
       </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>7.6999999999999957E-2</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>380</v>
       </c>
       <c r="B20">
@@ -3462,10 +3817,14 @@
       <c r="D20">
         <v>7.774</v>
       </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>-0.10899999999999999</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
       <c r="B21">
@@ -3477,6 +3836,10 @@
       <c r="D21">
         <v>7.7069999999999999</v>
       </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>-6.9999999999996732E-3</v>
+      </c>
       <c r="H21" t="s">
         <v>6</v>
       </c>
@@ -3489,7 +3852,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>420</v>
       </c>
       <c r="B22">
@@ -3500,6 +3863,10 @@
       </c>
       <c r="D22">
         <v>7.923</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>-0.20300000000000029</v>
       </c>
       <c r="G22" t="s">
         <v>4</v>
@@ -3519,7 +3886,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>440</v>
       </c>
       <c r="B23">
@@ -3530,6 +3897,10 @@
       </c>
       <c r="D23">
         <v>7.6989999999999998</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000021E-2</v>
       </c>
       <c r="G23" t="s">
         <v>5</v>
@@ -3549,7 +3920,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>460</v>
       </c>
       <c r="B24">
@@ -3561,10 +3932,14 @@
       <c r="D24">
         <v>7.6929999999999996</v>
       </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000021E-2</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>480</v>
       </c>
       <c r="B25">
@@ -3576,10 +3951,14 @@
       <c r="D25">
         <v>7.7350000000000003</v>
       </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>-9.2999999999999972E-2</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
       <c r="B26">
@@ -3591,10 +3970,14 @@
       <c r="D26">
         <v>7.7549999999999999</v>
       </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>-7.5999999999999623E-2</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>520</v>
       </c>
       <c r="B27">
@@ -3606,10 +3989,14 @@
       <c r="D27">
         <v>7.7640000000000002</v>
       </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>-9.7999999999999865E-2</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>540</v>
       </c>
       <c r="B28">
@@ -3621,10 +4008,14 @@
       <c r="D28">
         <v>7.72</v>
       </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>-6.9999999999996732E-3</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>560</v>
       </c>
       <c r="B29">
@@ -3636,10 +4027,14 @@
       <c r="D29">
         <v>7.6740000000000004</v>
       </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>9.5999999999999197E-2</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>580</v>
       </c>
       <c r="B30">
@@ -3651,10 +4046,21 @@
       <c r="D30">
         <v>7.673</v>
       </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>4.3999999999999595E-2</v>
+      </c>
+      <c r="G30" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30">
+        <f>AVERAGE(Table1[SUC - unSUC])</f>
+        <v>5.2739999999999988E-2</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>600</v>
       </c>
       <c r="B31">
@@ -3666,10 +4072,14 @@
       <c r="D31">
         <v>7.7629999999999999</v>
       </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0.15899999999999981</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>620</v>
       </c>
       <c r="B32">
@@ -3681,10 +4091,14 @@
       <c r="D32">
         <v>8.2070000000000007</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>-0.24500000000000099</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>640</v>
       </c>
       <c r="B33">
@@ -3696,10 +4110,14 @@
       <c r="D33">
         <v>8.1649999999999991</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>0.11300000000000132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>660</v>
       </c>
       <c r="B34">
@@ -3711,10 +4129,14 @@
       <c r="D34">
         <v>9.2360000000000007</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <f t="shared" ref="E34:E65" si="2">C34 - D34</f>
+        <v>0.35299999999999976</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>680</v>
       </c>
       <c r="B35">
@@ -3726,10 +4148,14 @@
       <c r="D35">
         <v>8.907</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>-0.92199999999999971</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>700</v>
       </c>
       <c r="B36">
@@ -3741,10 +4167,14 @@
       <c r="D36">
         <v>7.6849999999999996</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>9.0000000000000746E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>720</v>
       </c>
       <c r="B37">
@@ -3756,10 +4186,14 @@
       <c r="D37">
         <v>7.7160000000000002</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>8.8999999999999524E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>740</v>
       </c>
       <c r="B38">
@@ -3771,10 +4205,14 @@
       <c r="D38">
         <v>7.8140000000000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>-0.11099999999999977</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>760</v>
       </c>
       <c r="B39">
@@ -3786,10 +4224,14 @@
       <c r="D39">
         <v>7.7130000000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>-2.5000000000000355E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>780</v>
       </c>
       <c r="B40">
@@ -3801,10 +4243,14 @@
       <c r="D40">
         <v>7.7439999999999998</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>-4.9999999999999822E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>800</v>
       </c>
       <c r="B41">
@@ -3816,10 +4262,14 @@
       <c r="D41">
         <v>7.7190000000000003</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>2.7999999999999581E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>820</v>
       </c>
       <c r="B42">
@@ -3831,10 +4281,14 @@
       <c r="D42">
         <v>7.7619999999999996</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>-1.899999999999924E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>840</v>
       </c>
       <c r="B43">
@@ -3846,10 +4300,14 @@
       <c r="D43">
         <v>7.7619999999999996</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>-0.11199999999999921</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>860</v>
       </c>
       <c r="B44">
@@ -3861,10 +4319,14 @@
       <c r="D44">
         <v>7.7080000000000002</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>-6.0999999999999943E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>880</v>
       </c>
       <c r="B45">
@@ -3876,10 +4338,14 @@
       <c r="D45">
         <v>7.8230000000000004</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>-0.15600000000000058</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>900</v>
       </c>
       <c r="B46">
@@ -3891,10 +4357,14 @@
       <c r="D46">
         <v>7.681</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>9.0000000000003411E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>920</v>
       </c>
       <c r="B47">
@@ -3906,10 +4376,14 @@
       <c r="D47">
         <v>7.875</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>8.6000000000000298E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>940</v>
       </c>
       <c r="B48">
@@ -3921,10 +4395,14 @@
       <c r="D48">
         <v>7.7960000000000003</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>-0.12600000000000033</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>960</v>
       </c>
       <c r="B49">
@@ -3936,10 +4414,14 @@
       <c r="D49">
         <v>7.72</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>3.3999999999999808E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>980</v>
       </c>
       <c r="B50">
@@ -3951,10 +4433,14 @@
       <c r="D50">
         <v>7.774</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>-0.11000000000000032</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="B51">
@@ -3965,6 +4451,10 @@
       </c>
       <c r="D51">
         <v>7.7279999999999998</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>-6.1999999999999389E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the results to contain the Network Utlization test
</commit_message>
<xml_diff>
--- a/documents/encryption_test_results.xlsx
+++ b/documents/encryption_test_results.xlsx
@@ -908,11 +908,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="215461840"/>
-        <c:axId val="215455960"/>
+        <c:axId val="221933176"/>
+        <c:axId val="221928864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="215461840"/>
+        <c:axId val="221933176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1016,7 +1016,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="215455960"/>
+        <c:crossAx val="221928864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1024,7 +1024,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="215455960"/>
+        <c:axId val="221928864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="7"/>
@@ -1137,7 +1137,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="215461840"/>
+        <c:crossAx val="221933176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1664,11 +1664,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="215460664"/>
-        <c:axId val="215455568"/>
+        <c:axId val="221932392"/>
+        <c:axId val="221930432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="215460664"/>
+        <c:axId val="221932392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1779,7 +1779,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="215455568"/>
+        <c:crossAx val="221930432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1787,7 +1787,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="215455568"/>
+        <c:axId val="221930432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.13"/>
@@ -1900,7 +1900,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="215460664"/>
+        <c:crossAx val="221932392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4130,7 +4130,7 @@
         <v>9.2360000000000007</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E65" si="2">C34 - D34</f>
+        <f t="shared" ref="E34:E51" si="2">C34 - D34</f>
         <v>0.35299999999999976</v>
       </c>
     </row>

</xml_diff>